<commit_message>
Excel Item Master upload
</commit_message>
<xml_diff>
--- a/src/assets/files/ItemUpload.xlsx
+++ b/src/assets/files/ItemUpload.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Item Name</t>
   </si>
@@ -34,25 +34,22 @@
     <t>Good</t>
   </si>
   <si>
-    <t>Mobile</t>
-  </si>
-  <si>
     <t>Vendor Name</t>
-  </si>
-  <si>
-    <t>Location Code</t>
-  </si>
-  <si>
-    <t>kathir</t>
-  </si>
-  <si>
-    <t>trichy</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>Electronic</t>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Kannan</t>
+  </si>
+  <si>
+    <t>Madurai</t>
+  </si>
+  <si>
+    <t>Location Name</t>
   </si>
 </sst>
 </file>
@@ -248,7 +245,7 @@
     <tableColumn id="3" name="Item Category" dataDxfId="5"/>
     <tableColumn id="4" name="Item Description" dataDxfId="4"/>
     <tableColumn id="17" name="Vendor Name" dataDxfId="3"/>
-    <tableColumn id="5" name="Location Code" dataDxfId="2"/>
+    <tableColumn id="5" name="Location Name" dataDxfId="2"/>
     <tableColumn id="6" name="Opening Balance" dataDxfId="1"/>
     <tableColumn id="7" name="Default Price" dataDxfId="0"/>
   </tableColumns>
@@ -544,7 +541,7 @@
   <dimension ref="A1:AL997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -553,7 +550,7 @@
     <col min="2" max="2" width="16.7265625" customWidth="1"/>
     <col min="3" max="3" width="12.1796875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" customWidth="1"/>
+    <col min="5" max="5" width="17.54296875" customWidth="1"/>
     <col min="6" max="6" width="21.26953125" customWidth="1"/>
     <col min="7" max="7" width="14.453125" customWidth="1"/>
     <col min="8" max="8" width="13.54296875" customWidth="1"/>
@@ -582,10 +579,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>3</v>
@@ -596,10 +593,10 @@
     </row>
     <row r="2" spans="1:38">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
@@ -611,10 +608,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:38">

</xml_diff>